<commit_message>
endpoint and validation fixes
</commit_message>
<xml_diff>
--- a/project-evaluation.xlsx
+++ b/project-evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\Desktop\BLG317E-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102EA805-F0A1-4694-BE54-EB4F04E1470E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2A8B4F-5691-4B7A-A295-8A1537DC6B0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>Implemented live sorting</t>
   </si>
   <si>
-    <t>Included statistics</t>
-  </si>
-  <si>
     <t>Amazing Frontend</t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>Implemented scroll pagination due to the data being big . It was very hard</t>
+  </si>
+  <si>
+    <t>Included statistics by utilizing subqueries and functions and groupby</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1618,7 +1618,7 @@
         <v>32</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="44" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="16" t="s">
         <v>78</v>
@@ -1726,7 +1726,7 @@
         <v>81</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
@@ -1772,14 +1772,14 @@
     </row>
     <row r="48" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="8"/>
@@ -1789,10 +1789,10 @@
     </row>
     <row r="49" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -1804,10 +1804,10 @@
     </row>
     <row r="50" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -2017,12 +2017,13 @@
       <c r="H86" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B44:I44"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B48:E48"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>